<commit_message>
Implementation of Simplex algorithm
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/ElementaryPivotingTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/ElementaryPivotingTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="3"/>
+    <workbookView xWindow="8205" yWindow="2745" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="test 5x6 on 2,4" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -1950,1251 +1950,1251 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*20-7</f>
-        <v>-0.43638794775312562</v>
+        <v>7.8668144396763608</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:L16" ca="1" si="0">RAND()*20-7</f>
-        <v>8.1201321209878099</v>
+        <v>-5.3734727769572999</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9208326755475085</v>
+        <v>10.665120038529125</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>7.6938236503678361</v>
+        <v>-3.1862158250977739</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>11.2151747172692</v>
+        <v>7.7369446986446171</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3605476982659006</v>
+        <v>1.901821398562257</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4728469983961361</v>
+        <v>8.2351544251678028</v>
       </c>
       <c r="H1">
         <f t="shared" ca="1" si="0"/>
-        <v>8.749123731855299</v>
+        <v>5.7427431265239726</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8105035136797518</v>
+        <v>-5.299329066721441</v>
       </c>
       <c r="J1">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.7469401867340419</v>
+        <v>0.66865822487080528</v>
       </c>
       <c r="K1">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.783262109621917</v>
+        <v>3.5595635448355463</v>
       </c>
       <c r="L1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1096839184037437</v>
+        <v>3.7331028931890398</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:L25" ca="1" si="1">RAND()*20-7</f>
-        <v>4.9737012988603198</v>
+        <v>-4.725193842690703</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8519192062617087</v>
+        <v>10.314508968497218</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3039068229875319</v>
+        <v>-3.0327017726722953</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>11.065614865874686</v>
+        <v>11.5822204205883</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7881922388510993</v>
+        <v>-0.6118579033070608</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.140769446943235</v>
+        <v>8.203687825814109</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3612475953741416</v>
+        <v>-3.8240578191204082</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>10.437510398004655</v>
+        <v>-4.4508596324983456</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.22295987875242851</v>
+        <v>-5.9329880636952907</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>10.829890276269531</v>
+        <v>-3.8588336307997122</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3912313300197976</v>
+        <v>-4.1679906824017081</v>
       </c>
       <c r="L2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8704419790924476</v>
+        <v>3.1610282432098469</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.2063183697303099</v>
+        <v>0.45561211555646697</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7869190837055058</v>
+        <v>0.41564928711325511</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.15732880900283774</v>
+        <v>7.0984997516911505</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3960664866685022</v>
+        <v>-4.8819046613187211</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.0669422940938507</v>
+        <v>3.3819735864217897</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>10.050801829362563</v>
+        <v>5.2028701159472099</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.484568968214953</v>
+        <v>1.6031355906472324</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.1258043441788903</v>
+        <v>-2.2725249118880502</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.01693407674518</v>
+        <v>-4.8138415144298312</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.2493976394922566</v>
+        <v>-1.5494987967906342</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2381089233305413</v>
+        <v>4.4443313834024565</v>
       </c>
       <c r="L3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3948157566116102</v>
+        <v>4.3148685517052794</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24570067220387859</v>
+        <v>1.909655205952987E-2</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.79222184702243048</v>
+        <v>3.5798252874638017</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>8.8727533468771913</v>
+        <v>-0.92331690876692107</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.0336878738791433</v>
+        <v>-6.8087579420611632</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.4601245543522001</v>
+        <v>11.462808629554043</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.2804833374953102</v>
+        <v>0.59374917284318496</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.7175742286469919</v>
+        <v>-6.6393468957120927</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>9.9886058866237413</v>
+        <v>-5.6160362373515671</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>10.914564580743175</v>
+        <v>10.681300462041417</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7909361535541564</v>
+        <v>-6.5291310589714628</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3094342559759351</v>
+        <v>-1.3707951107009668</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6793724003472708</v>
+        <v>-1.1137323656218232</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1262665163897214</v>
+        <v>0.68725319179638156</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.7198222109064432</v>
+        <v>-4.2158057415053261</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>9.0093447849785484</v>
+        <v>5.6641878915889947</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.8387933482436729</v>
+        <v>-2.2055694890677318</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1049175854323483</v>
+        <v>-1.2758959577783839</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.2818767509513229</v>
+        <v>-4.9685486982441649</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1203141506217413</v>
+        <v>-6.6240015093141658</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7843906201189235</v>
+        <v>4.102096482232394</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>12.190220151556353</v>
+        <v>-2.7549696556563834</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.1763167653055149</v>
+        <v>0.95737927278821822</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.2295377255648643</v>
+        <v>7.7767263604629466</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="0"/>
-        <v>12.11698250831715</v>
+        <v>9.7895259297103898</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.4808233980129053</v>
+        <v>12.097876157270541</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0245817703421842</v>
+        <v>11.169018678864585</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4387726909720762</v>
+        <v>12.05642202733539</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>7.6203409867520442</v>
+        <v>12.965791857124941</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>12.325843719848397</v>
+        <v>8.9250619786340035</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3316591124414217</v>
+        <v>-6.2287240264399273</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.6493052543699562</v>
+        <v>1.2922790861572899</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3079775715285713</v>
+        <v>-0.50742883530870309</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9699111176220292</v>
+        <v>7.3608127228922413</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>8.3062390019060679</v>
+        <v>3.3822685738540681</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7086950296913788</v>
+        <v>-6.8977815673497149</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9228764525411428</v>
+        <v>-4.5453495907649586</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.9856017280505025</v>
+        <v>11.307960065189409</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1487606175095912</v>
+        <v>2.3830111378219669</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>11.434595540994373</v>
+        <v>11.441222703781794</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>10.171516227393656</v>
+        <v>10.415276244869936</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2334065463808308</v>
+        <v>6.2610930523331287</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2786501784246056</v>
+        <v>-3.8419877073410285</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.55594345690503921</v>
+        <v>11.445432858478512</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>8.3882905522796261</v>
+        <v>8.6646713397196748</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3941329844528383</v>
+        <v>11.829212374708792</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0190973427820911</v>
+        <v>-6.6577888159228316</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.89933576332070331</v>
+        <v>7.9215225045096673</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.3539979332274577</v>
+        <v>7.964782471132045</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>11.175896266638599</v>
+        <v>11.405161836726961</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>12.314073280961203</v>
+        <v>-0.2821177657791889</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>11.116393120893402</v>
+        <v>-4.0529159585469365</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9121811130053654</v>
+        <v>-1.590899909432153</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>11.10817706832389</v>
+        <v>-3.7423138896976531</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.7984871962851585</v>
+        <v>10.441826902987639</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>11.945540373460126</v>
+        <v>6.1672244490454595</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.572437650740099</v>
+        <v>-0.8681099246513746</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>9.0908127608467808</v>
+        <v>12.526977590136024</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.558888983079088</v>
+        <v>0.49360077130140745</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.0187622781551333</v>
+        <v>-0.68804624098267375</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4322156116379414</v>
+        <v>-6.2058157870038038</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.10374826204907972</v>
+        <v>6.1296621696503539</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>7.6575667883478555</v>
+        <v>9.0337579899566194</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4680236021451005</v>
+        <v>3.8689395154364892</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.0932977899098475</v>
+        <v>-3.8939346769154142</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30662121864945213</v>
+        <v>-5.3042513155668001</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>11.054763221489793</v>
+        <v>0.9679101384701756</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>7.9651849854328045</v>
+        <v>10.470413267306284</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>4.6579572551071013</v>
+        <v>9.8705245283295859</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1883444302143218</v>
+        <v>10.347140161645974</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5232523917781613</v>
+        <v>6.6630551658499932</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="0"/>
-        <v>8.4883864167746399</v>
+        <v>-2.9366643804592361</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.917161286437187</v>
+        <v>-0.30951874333153206</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2171593602093882</v>
+        <v>-4.4384191291297235</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1103613682413389</v>
+        <v>-5.1792420737579752</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.6941912057039001</v>
+        <v>8.5014277821145985</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.0871033163156998</v>
+        <v>-0.19515655048524305</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7673335529407694</v>
+        <v>7.6826338775512042</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6345960371335249</v>
+        <v>1.4910993964241737</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>6.696757386885551</v>
+        <v>1.7602186992145885</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>1.45037971834582</v>
+        <v>2.2904325205117608</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.52956188828095918</v>
+        <v>4.2561313365504105</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7525128994051684</v>
+        <v>-6.3218212842595261</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7407192528095994</v>
+        <v>8.1339491066451419</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="0"/>
-        <v>12.499843493177362</v>
+        <v>0.91729482332434742</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5417806517130543</v>
+        <v>7.4273078348801391</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.2861038169667207</v>
+        <v>11.475990299531265</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5702460863637384</v>
+        <v>-1.2642792485688785</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3478864052381674</v>
+        <v>-0.42016332005672652</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2154134976775364</v>
+        <v>10.685719447419743</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>9.0288610758792451</v>
+        <v>11.315351878222252</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7872275980872576</v>
+        <v>3.2326974534562147</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.0890283178842153</v>
+        <v>0.13457873023011224</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>8.4024759992281606</v>
+        <v>8.0140103422403843</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>12.533079430365337</v>
+        <v>-2.3166046570333725</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="0"/>
-        <v>11.319048968773327</v>
+        <v>-0.23539745288781155</v>
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6646295809016074</v>
+        <v>12.538597034752637</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>11.99212718780954</v>
+        <v>7.2644952483528353</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.2798516123077377</v>
+        <v>5.5306908690275325</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.555804145849681</v>
+        <v>3.2700996362203583</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>12.106573260599042</v>
+        <v>6.3816477060098933</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7447110478683037</v>
+        <v>-0.98142301067074378</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3427229550890587</v>
+        <v>-4.2308513845024454</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>8.0399078538186632</v>
+        <v>12.500077522241178</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7172212796223079</v>
+        <v>-2.7494585638799727</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1998572878543587</v>
+        <v>11.314460954281074</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.0266439196613208</v>
+        <v>3.6015594849059998</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.7131120547594607</v>
+        <v>12.727372453979875</v>
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="0"/>
-        <v>7.9692803207203902</v>
+        <v>8.04322950472047</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2449553894120857</v>
+        <v>9.9749582100265499</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>9.6721054232784454</v>
+        <v>10.345429787037066</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.9392897619409641</v>
+        <v>-2.0941967519240023</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.9460101483903767</v>
+        <v>11.527431195858203</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8540764853304736</v>
+        <v>-4.8783157046904524</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.9283540369270007</v>
+        <v>9.9601538186071537</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.3761039186839454</v>
+        <v>12.322216963884305</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.0492008110571058</v>
+        <v>-3.6600000233541001</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2774391797926796</v>
+        <v>7.5131160432710011</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>8.1961224184307966</v>
+        <v>-6.3981487689605174</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="0"/>
-        <v>11.29815014634621</v>
+        <v>6.844511894844814</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5290683532334626</v>
+        <v>-3.891686034773663</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5472286246487243</v>
+        <v>-5.5309046981378174</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2331274513130008</v>
+        <v>-6.5578838961067021</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>10.650818292712067</v>
+        <v>8.4068094646080151</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>9.771689834230223</v>
+        <v>9.0667834447129216</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5822861500630978</v>
+        <v>-4.446713423909177</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1098321273558369</v>
+        <v>-3.8963556055233033</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>4.876282373655183E-2</v>
+        <v>-0.39242049110108468</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>10.20554790189237</v>
+        <v>6.1398621993867479</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.5056169393501442</v>
+        <v>1.5297850238688877</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>12.615885032467048</v>
+        <v>-3.7686107832871878</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82099664067862577</v>
+        <v>-2.4396666024337836</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9043090801955991</v>
+        <v>9.0927643066370436</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.3799267776602093</v>
+        <v>-5.4646222544867911</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1991111122065963</v>
+        <v>11.133029018906292</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5269363141121204</v>
+        <v>0.44554029669883555</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29148114910367973</v>
+        <v>-1.9657340740463951</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1040017646780864</v>
+        <v>3.0607330805682693</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.7585022305261688</v>
+        <v>3.0898894559792307</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>11.620061094339956</v>
+        <v>2.7571840574365982</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>12.293230213822316</v>
+        <v>10.263021554326631</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1749593850819364</v>
+        <v>8.4069190845002186</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>9.0883561644697011</v>
+        <v>3.2682014999135411</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.7926848083050277</v>
+        <v>6.9511758743375864</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="0"/>
-        <v>6.117484606177463</v>
+        <v>12.032282584126371</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>9.2142882452743393</v>
+        <v>5.9481967296681155</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46392644826647356</v>
+        <v>6.0053905483498582</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8426370967455643</v>
+        <v>5.4887501642428038</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1243308601216526</v>
+        <v>0.11837287658132212</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.2533735592332986</v>
+        <v>8.0394981333021995</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>8.1642371782871876</v>
+        <v>3.4450494811149053</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>6.305033503863136</v>
+        <v>-0.12942771260411767</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7367100913665965</v>
+        <v>12.633951909514796</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.0238550793796595</v>
+        <v>7.0287407204074697</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9056916678958586</v>
+        <v>2.6486615319360389</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="0"/>
-        <v>11.079690002186759</v>
+        <v>12.053703293563139</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8297259250089919</v>
+        <v>2.7629582196275688</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4955206016674616</v>
+        <v>6.8025410696535484</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3622533149944278</v>
+        <v>8.3452195394948614</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0749338673529767</v>
+        <v>0.12521734572528587</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.2487399035845828</v>
+        <v>-4.1867561776666156</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6034972622490535</v>
+        <v>3.1953937969447406</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>4.6188629111308082</v>
+        <v>5.3394187884595183</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.0537303979275396</v>
+        <v>-2.8725324619620949</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>10.028821888919893</v>
+        <v>5.5650930441096627</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>7.9541125869429141</v>
+        <v>2.1074471801578447</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5415806519594994</v>
+        <v>3.7779643211623277</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.73756598708566834</v>
+        <v>-1.466107042446799</v>
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="1"/>
-        <v>7.8624828243624201</v>
+        <v>1.1444053319649239</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>8.9335408595617363</v>
+        <v>2.2463177670995655</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.2892476203394496</v>
+        <v>3.2105343983947101</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5361730017750546</v>
+        <v>-0.51323023796091594</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>6.7253016056473687</v>
+        <v>-3.8799569154373863</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0472118568624786</v>
+        <v>5.8763171698849899</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>11.359623160926169</v>
+        <v>8.1658745223887195</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.4844301311922994</v>
+        <v>-4.1133355337831965</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.373040699604509</v>
+        <v>11.115276963801175</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>8.7850861070969621</v>
+        <v>-6.2439295474724741</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.8214292599988635</v>
+        <v>11.320242581276766</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="1"/>
-        <v>5.0420954552400179</v>
+        <v>-1.5020288855859398</v>
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="1"/>
-        <v>11.088588915818342</v>
+        <v>-4.3179710522360182</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4032691242645843</v>
+        <v>3.4184388040909255</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.4489869283340209</v>
+        <v>-4.3145126504097728</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3040468670149075</v>
+        <v>-2.1788973764387176</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>9.5475328200792013</v>
+        <v>4.2336637457759245</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.1574201773863848</v>
+        <v>-2.3251332042790374</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.8427027679802048</v>
+        <v>0.61123766203452679</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0466440932648808</v>
+        <v>-2.7238027642003804</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.048161960685503</v>
+        <v>10.685984710744385</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18738380708870039</v>
+        <v>4.1472802716498656</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.4179374140237222</v>
+        <v>-0.48106518792432418</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.6102963378818549</v>
+        <v>-2.7812382930743622</v>
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="1"/>
-        <v>7.8785456588422846</v>
+        <v>3.1869165774082582</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.1508339579147258</v>
+        <v>-1.690460178020734</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>5.0029509338926843</v>
+        <v>4.6487824290179915</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>12.982312195593607</v>
+        <v>8.9454311173179608</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.6850948999547679</v>
+        <v>-3.1627845572723361</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>6.8591423335018931</v>
+        <v>10.762762853650937</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.7845127456027576</v>
+        <v>-3.759660956851079</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.5254615845334092</v>
+        <v>7.8698262615410179</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>9.6444156787422806</v>
+        <v>-3.8098647264614054</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>4.23142033662511</v>
+        <v>9.4851143165208534</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="1"/>
-        <v>12.169002811314915</v>
+        <v>4.8410730109494153</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="1"/>
-        <v>6.9322509649559798</v>
+        <v>3.4410463199436538</v>
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.8293614168635859</v>
+        <v>-0.57732087606622073</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>7.9224952477651858</v>
+        <v>1.4164683910094062</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5255044727500877</v>
+        <v>4.2379587528247029</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>12.698710043986697</v>
+        <v>10.475709987151962</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5450031484779423</v>
+        <v>11.044971509263451</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>12.481735337823164</v>
+        <v>8.7826567323330131</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1210826292979768</v>
+        <v>6.8329816725306625</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3760777223491232</v>
+        <v>5.6787447882799214</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.6861904679991939</v>
+        <v>-0.85132853264287434</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.7823290696312153</v>
+        <v>-4.251322710473258</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1841312914494289</v>
+        <v>12.927417179520056</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="1"/>
-        <v>7.6090580130161545</v>
+        <v>-0.53764446605865857</v>
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="1"/>
-        <v>8.392384155701702</v>
+        <v>7.6890701810419095</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.4332471372464006</v>
+        <v>10.848642811374191</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76075010688377631</v>
+        <v>9.0063789668277785</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3639413836716106</v>
+        <v>-1.2364371294716507</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>6.8801218727363658</v>
+        <v>2.5529108886382126</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.7560004704664411</v>
+        <v>7.7260287558369107</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.5693219129059814</v>
+        <v>12.934151593590961</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4353623971095217</v>
+        <v>11.519285303638679</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>12.605104036688626</v>
+        <v>-4.476607964486675</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.9829567893576305</v>
+        <v>-2.1263224991554868</v>
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.8602179956098972</v>
+        <v>9.8900595708356747</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="1"/>
-        <v>12.549916410551887</v>
+        <v>5.7970767019514362</v>
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27728486202032165</v>
+        <v>5.7999435317814871</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3025156652958003</v>
+        <v>-2.9840640681288626</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8896990330571661</v>
+        <v>7.3172315510526342</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.8442142803613155</v>
+        <v>6.3240941758500657</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.9844611491549298</v>
+        <v>-4.0437033573191643</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3655118469325132</v>
+        <v>9.5961763740888486</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0284825837814839</v>
+        <v>3.8108517890857563E-2</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>6.328947205588797</v>
+        <v>3.6827316159243431</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>11.642471270297712</v>
+        <v>3.2497460078078682</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5400965753953404</v>
+        <v>-4.523270478176074</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3922901441426205</v>
+        <v>3.2857838399584427</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3141113370496988</v>
+        <v>4.1154194422801602</v>
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.276609840073661</v>
+        <v>-4.8498957149706383</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.529535258232475</v>
+        <v>10.701044998256261</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.75872711972433127</v>
+        <v>3.5380623311018606</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1428492844415423</v>
+        <v>10.135878532548215</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>12.929836634249554</v>
+        <v>-1.1117494416269622</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>11.33421301795266</v>
+        <v>11.51774387992339</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.1989388039188302</v>
+        <v>4.7017726309459604</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2798978540025931</v>
+        <v>2.0138474603526575</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9756517600820906</v>
+        <v>-3.7596283818303027</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
-        <v>2.481997094387058</v>
+        <v>2.0512369815925879</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76299776038356537</v>
+        <v>-3.7770490863004706</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0268187476920296</v>
+        <v>-5.9016024650266701</v>
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9214187187643272</v>
+        <v>3.1947582796624641</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.5651603513364485</v>
+        <v>-2.8216022890295349</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>12.992172740785939</v>
+        <v>7.4955726364938329</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>11.774754379010389</v>
+        <v>2.868367327168448</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.40044707443420524</v>
+        <v>3.6982542097572946</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.5226614719293465</v>
+        <v>-2.9210217740603799</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>10.034779242976818</v>
+        <v>-4.6968353352533097</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.46773472842990493</v>
+        <v>5.0011768077839349</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.3437323717634744</v>
+        <v>7.0483213262991171</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1904078093916759</v>
+        <v>11.456684131875441</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4444019498786709</v>
+        <v>-2.5925478371670874</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.7143272762454576</v>
+        <v>3.9024574561706054</v>
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.2931398798566107</v>
+        <v>-4.4802708575672439</v>
       </c>
     </row>
   </sheetData>
@@ -3206,7 +3206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>